<commit_message>
Cafe de los maestros Eintritt und Kiosk eingetragen
</commit_message>
<xml_diff>
--- a/Input/Spezialpreisekiosk.xlsx
+++ b/Input/Spezialpreisekiosk.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Kinoklub\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F475D00A-A51E-4B32-ACB3-15A9B438193F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ED4C008-923A-4BB0-9736-E258EBEAEE8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="18696" xr2:uid="{5CFCAA73-5DB4-4EB4-81C9-1C9C0D98D4AD}"/>
+    <workbookView xWindow="2964" yWindow="1884" windowWidth="15684" windowHeight="11832" xr2:uid="{5CFCAA73-5DB4-4EB4-81C9-1C9C0D98D4AD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="30">
   <si>
     <t>Datum</t>
   </si>
@@ -123,6 +123,9 @@
   </si>
   <si>
     <t>Zaubertrank</t>
+  </si>
+  <si>
+    <t>Rotwein</t>
   </si>
 </sst>
 </file>
@@ -190,8 +193,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9A44B4B4-A546-4A04-B7DF-39B4610A3FD4}" name="Table1" displayName="Table1" ref="A1:E29" totalsRowShown="0">
-  <autoFilter ref="A1:E29" xr:uid="{9A44B4B4-A546-4A04-B7DF-39B4610A3FD4}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9A44B4B4-A546-4A04-B7DF-39B4610A3FD4}" name="Table1" displayName="Table1" ref="A1:E30" totalsRowShown="0">
+  <autoFilter ref="A1:E30" xr:uid="{9A44B4B4-A546-4A04-B7DF-39B4610A3FD4}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{2E4FAC83-4FC6-4E6F-87B3-8377FC66120C}" name="Datum" dataDxfId="1"/>
     <tableColumn id="2" xr3:uid="{7C6D28F5-89B2-4342-9089-E87764A5F47F}" name="Spezialpreis"/>
@@ -500,10 +503,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD21FE1F-65EF-43DF-AD1F-FCA81656A71F}">
-  <dimension ref="A1:E29"/>
+  <dimension ref="A1:E30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1008,6 +1011,20 @@
         <v>1</v>
       </c>
     </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A30" s="1">
+        <v>45626</v>
+      </c>
+      <c r="B30" t="s">
+        <v>5</v>
+      </c>
+      <c r="C30" t="s">
+        <v>29</v>
+      </c>
+      <c r="D30" s="2">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
Filmvorführung Buchspazierer 20.12.24 Eintritte und Kiosk
</commit_message>
<xml_diff>
--- a/Input/Spezialpreisekiosk.xlsx
+++ b/Input/Spezialpreisekiosk.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Kinoklub\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AF0EFDA-9E71-4EE4-9B0C-FBD3A3D194F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7D0D4DB-BE98-45C0-ACA3-F363E150A217}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3312" yWindow="2232" windowWidth="15684" windowHeight="11832" xr2:uid="{5CFCAA73-5DB4-4EB4-81C9-1C9C0D98D4AD}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="18696" xr2:uid="{5CFCAA73-5DB4-4EB4-81C9-1C9C0D98D4AD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="38">
   <si>
     <t>Datum</t>
   </si>
@@ -144,6 +144,12 @@
   </si>
   <si>
     <t>Raclette - Schnitte</t>
+  </si>
+  <si>
+    <t>Weisswein</t>
+  </si>
+  <si>
+    <t>Buch: Buchspazierer</t>
   </si>
 </sst>
 </file>
@@ -211,8 +217,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9A44B4B4-A546-4A04-B7DF-39B4610A3FD4}" name="Table1" displayName="Table1" ref="A1:E36" totalsRowShown="0">
-  <autoFilter ref="A1:E36" xr:uid="{9A44B4B4-A546-4A04-B7DF-39B4610A3FD4}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9A44B4B4-A546-4A04-B7DF-39B4610A3FD4}" name="Table1" displayName="Table1" ref="A1:E39" totalsRowShown="0">
+  <autoFilter ref="A1:E39" xr:uid="{9A44B4B4-A546-4A04-B7DF-39B4610A3FD4}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{2E4FAC83-4FC6-4E6F-87B3-8377FC66120C}" name="Datum" dataDxfId="1"/>
     <tableColumn id="2" xr3:uid="{7C6D28F5-89B2-4342-9089-E87764A5F47F}" name="Spezialpreis"/>
@@ -521,10 +527,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD21FE1F-65EF-43DF-AD1F-FCA81656A71F}">
-  <dimension ref="A1:E36"/>
+  <dimension ref="A1:E39"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="A37" sqref="A37"/>
+      <selection activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1127,6 +1133,48 @@
         <v>4</v>
       </c>
     </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A37" s="1">
+        <v>45646</v>
+      </c>
+      <c r="B37" t="s">
+        <v>5</v>
+      </c>
+      <c r="C37" t="s">
+        <v>29</v>
+      </c>
+      <c r="D37" s="2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A38" s="1">
+        <v>45646</v>
+      </c>
+      <c r="B38" t="s">
+        <v>6</v>
+      </c>
+      <c r="C38" t="s">
+        <v>36</v>
+      </c>
+      <c r="D38" s="2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A39" s="1">
+        <v>45646</v>
+      </c>
+      <c r="B39" t="s">
+        <v>10</v>
+      </c>
+      <c r="C39" t="s">
+        <v>37</v>
+      </c>
+      <c r="D39" s="2">
+        <v>23.5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
Eintritte, Kiosk und spezpreis angepasst für Flow 19.01.25
</commit_message>
<xml_diff>
--- a/Input/Spezialpreisekiosk.xlsx
+++ b/Input/Spezialpreisekiosk.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\R Packages\Kinoklub\Input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Kinoklub\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD031016-809E-422A-9775-E576C1B1870F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EB27B8E-7693-4C68-A725-4EEA05E127B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{5CFCAA73-5DB4-4EB4-81C9-1C9C0D98D4AD}"/>
+    <workbookView xWindow="15264" yWindow="0" windowWidth="15552" windowHeight="18576" xr2:uid="{5CFCAA73-5DB4-4EB4-81C9-1C9C0D98D4AD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Datum</t>
   </si>
@@ -53,10 +53,7 @@
     <t>Spez 1</t>
   </si>
   <si>
-    <t>Leibniz Kekse Dschungel</t>
-  </si>
-  <si>
-    <t>Zaubertrank</t>
+    <t>Zuckerwatte</t>
   </si>
 </sst>
 </file>
@@ -101,7 +98,7 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
@@ -140,9 +137,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 – 2022-Design">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 – 2022">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -180,7 +177,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 – 2022">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -286,7 +283,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 – 2022">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -436,21 +433,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD21FE1F-65EF-43DF-AD1F-FCA81656A71F}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="14.7109375" customWidth="1"/>
-    <col min="3" max="3" width="17.28515625" customWidth="1"/>
-    <col min="4" max="4" width="16.42578125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="14.109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="14.6640625" customWidth="1"/>
+    <col min="3" max="3" width="17.33203125" customWidth="1"/>
+    <col min="4" max="4" width="14.6640625" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -464,9 +461,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
-        <v>45748</v>
+        <v>45676</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
@@ -475,20 +472,6 @@
         <v>5</v>
       </c>
       <c r="D2" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>45964</v>
-      </c>
-      <c r="B3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="2">
         <v>3</v>
       </c>
     </row>

</xml_diff>